<commit_message>
Add report and fix yi in MatProg lab2
</commit_message>
<xml_diff>
--- a/MatProg/Lab2/Lab2.xlsx
+++ b/MatProg/Lab2/Lab2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4606525E-C314-47B7-9C09-FA04AAD2B19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FFC074-1391-4465-A08A-6B66A484D569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Графически" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
   <si>
     <t>Ресурсы</t>
   </si>
@@ -1121,9 +1121,6 @@
   </si>
   <si>
     <t>y5</t>
-  </si>
-  <si>
-    <t>y6</t>
   </si>
   <si>
     <t>y1</t>
@@ -1145,12 +1142,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1258,7 +1263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1274,31 +1279,31 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1641,152 +1646,152 @@
       <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="9"/>
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9">
         <v>2</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9"/>
       <c r="N3" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="9">
         <v>1000</v>
       </c>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="9"/>
       <c r="N4" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="9">
         <v>500</v>
       </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1">
         <v>1200</v>
       </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8">
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="9"/>
       <c r="N5" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="9">
         <v>1200</v>
       </c>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
         <v>50</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
         <v>40</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="N6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1796,28 +1801,28 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1829,155 +1834,155 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:J25"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="N1" s="7" t="s">
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="9"/>
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="9">
         <v>1</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9">
         <v>2</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="9"/>
       <c r="N3" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="8">
+      <c r="P3" s="9">
         <v>1000</v>
       </c>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="9"/>
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
         <v>1</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="9"/>
       <c r="N4" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="8">
+      <c r="P4" s="9">
         <v>500</v>
       </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="1">
         <v>1200</v>
       </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8">
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
         <v>1</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="9"/>
       <c r="N5" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="8">
+      <c r="P5" s="9">
         <v>1200</v>
       </c>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
         <v>50</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
         <v>40</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="N6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1985,25 +1990,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N8" s="7" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -2035,12 +2040,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
       <c r="F10" s="1">
         <v>50</v>
       </c>
@@ -2064,16 +2069,16 @@
       <c r="O10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P10" s="8">
+      <c r="P10" s="9">
         <v>1000</v>
       </c>
-      <c r="Q10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="14">
-        <v>0</v>
-      </c>
-      <c r="B11" s="14"/>
+      <c r="Q10" s="9"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="11">
+        <v>0</v>
+      </c>
+      <c r="B11" s="11"/>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2101,25 +2106,25 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="13">
         <f>E11/F11</f>
         <v>1000</v>
       </c>
-      <c r="L11" s="11"/>
+      <c r="L11" s="13"/>
       <c r="N11" t="s">
         <v>21</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="8">
+      <c r="P11" s="9">
         <v>500</v>
       </c>
-      <c r="Q11" s="8"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
+      <c r="Q11" s="9"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2147,25 +2152,25 @@
       <c r="J12" s="3">
         <v>0</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="13">
         <f>E12/F12</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="L12" s="11"/>
+      <c r="L12" s="13"/>
       <c r="N12" t="s">
         <v>22</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="8">
+      <c r="P12" s="9">
         <v>1200</v>
       </c>
-      <c r="Q12" s="8"/>
-    </row>
-    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
+      <c r="Q12" s="9"/>
+    </row>
+    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2193,10 +2198,10 @@
       <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="K13" s="13" t="s">
+      <c r="K13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="13"/>
+      <c r="L13" s="14"/>
       <c r="N13" s="1" t="s">
         <v>17</v>
       </c>
@@ -2204,13 +2209,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="9" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="9"/>
+      <c r="D14" s="8"/>
       <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
@@ -2229,14 +2234,14 @@
       <c r="J14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
       <c r="E15" s="1">
         <v>0</v>
       </c>
@@ -2260,14 +2265,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="14">
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="11">
         <v>1</v>
       </c>
-      <c r="B16" s="14"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -2297,15 +2302,15 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="13">
         <f>E16/G16</f>
         <v>500</v>
       </c>
-      <c r="L16" s="11"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
@@ -2335,15 +2340,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="13">
         <f>E17/G17</f>
         <v>500</v>
       </c>
-      <c r="L17" s="11"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="14"/>
+      <c r="L17" s="13"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2373,26 +2378,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="13">
         <f>E18/G18</f>
         <v>1200</v>
       </c>
-      <c r="L18" s="11"/>
-      <c r="N18" s="10" t="s">
+      <c r="L18" s="13"/>
+      <c r="N18" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="9" t="s">
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="9"/>
+      <c r="D19" s="8"/>
       <c r="E19" s="2" t="s">
         <v>36</v>
       </c>
@@ -2411,19 +2416,19 @@
       <c r="J19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="1">
         <f>(E15*$F$12-$F15*E12)/$F$12</f>
         <v>8333.3333333333339</v>
@@ -2448,19 +2453,19 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11">
         <v>2</v>
       </c>
-      <c r="B21" s="14"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
@@ -2490,19 +2495,19 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K21" s="11" t="s">
+      <c r="K21" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="11"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="14"/>
+      <c r="L21" s="13"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2532,19 +2537,19 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="K22" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="11"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="14"/>
+      <c r="L22" s="13"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2574,23 +2579,23 @@
         <f>(J18*$G$16-J16*$G18)/$G$16</f>
         <v>1</v>
       </c>
-      <c r="K23" s="11" t="s">
+      <c r="K23" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="11"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="9" t="s">
+      <c r="L23" s="13"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="8"/>
       <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2609,19 +2614,19 @@
       <c r="J24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
       <c r="E25" s="5">
         <f>(E20*$G$16-E16*$G20)/$G$16</f>
         <v>20000</v>
@@ -2646,22 +2651,22 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -2670,28 +2675,18 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="N18:R25"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L25"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L20"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
     <mergeCell ref="A11:B15"/>
     <mergeCell ref="A16:B20"/>
     <mergeCell ref="A21:B25"/>
@@ -2708,332 +2703,6 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L20"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="N18:R25"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L25"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB38E0-1495-427A-B70D-7D750FA7B82B}">
-  <dimension ref="A1:Q22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="N1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="N2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="8"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="8">
-        <v>1</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8">
-        <v>2</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="8">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="8"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="1">
-        <v>500</v>
-      </c>
-      <c r="D4" s="8">
-        <v>3</v>
-      </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="N4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="8">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="8"/>
-    </row>
-    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="1">
-        <v>1200</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="N5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="8"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
-        <v>50</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8">
-        <v>40</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>20000</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="E15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A9:G10"/>
-    <mergeCell ref="A15:C22"/>
-    <mergeCell ref="E15:G22"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
@@ -3059,4 +2728,336 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB38E0-1495-427A-B70D-7D750FA7B82B}">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="14" max="14" width="16.109375" customWidth="1"/>
+    <col min="17" max="17" width="17.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="N1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="9"/>
+      <c r="N2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="9"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="9">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9">
+        <v>2</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="9">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="9"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="1">
+        <v>500</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="9">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="9"/>
+    </row>
+    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="N5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9">
+        <v>50</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9">
+        <v>40</v>
+      </c>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A12" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="E15" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="15"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="15"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="A9:G10"/>
+    <mergeCell ref="A15:C22"/>
+    <mergeCell ref="E15:G22"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fix to lab2 MatProg
</commit_message>
<xml_diff>
--- a/MatProg/Lab2/Lab2.xlsx
+++ b/MatProg/Lab2/Lab2.xlsx
@@ -1,22 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Labs\semester_5\MatProg\Lab2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FFC074-1391-4465-A08A-6B66A484D569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CE1CAC-B5A1-4C06-A6E0-3F95A411F2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Графически" sheetId="1" r:id="rId1"/>
     <sheet name="Симплекс-метод" sheetId="2" r:id="rId2"/>
     <sheet name="Двойственная задача" sheetId="3" r:id="rId3"/>
+    <sheet name="Отчет о результатах 1" sheetId="6" r:id="rId4"/>
+    <sheet name="Отчет об устойчивости 1" sheetId="7" r:id="rId5"/>
+    <sheet name="Отчет о пределах 1" sheetId="8" r:id="rId6"/>
+    <sheet name="Программное решение" sheetId="5" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="6" hidden="1">'Программное решение'!$B$3:$C$3</definedName>
+    <definedName name="solver_cvg" localSheetId="6" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="6" hidden="1">'Программное решение'!$E$8:$E$10</definedName>
+    <definedName name="solver_mip" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="6" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="6" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="6" hidden="1">'Программное решение'!$D$4</definedName>
+    <definedName name="solver_pre" localSheetId="6" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="6" hidden="1">'Программное решение'!$G$8:$G$10</definedName>
+    <definedName name="solver_rlx" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="5" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="6" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="6" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="6" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="6" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="6" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="6" hidden="1">3</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="128">
   <si>
     <t>Ресурсы</t>
   </si>
@@ -1136,13 +1173,223 @@
   </si>
   <si>
     <t>Также, согласно полученным данным, при увеличении ресурса P1 на 1 прибыль вырастет на y1=14, в то время как при увеличении ресурса P2 на 1 прибыль вырастет на y2=12</t>
+  </si>
+  <si>
+    <t>Переменные</t>
+  </si>
+  <si>
+    <t>имя</t>
+  </si>
+  <si>
+    <t>знач.</t>
+  </si>
+  <si>
+    <t>коэф. цел. ф.</t>
+  </si>
+  <si>
+    <t>Значение целевой функции</t>
+  </si>
+  <si>
+    <t>Ограничения</t>
+  </si>
+  <si>
+    <t>Вид</t>
+  </si>
+  <si>
+    <t>лев.ч.</t>
+  </si>
+  <si>
+    <t>знак</t>
+  </si>
+  <si>
+    <t>пр.ч.</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет о результатах</t>
+  </si>
+  <si>
+    <t>Лист: [Lab2.xlsx]Программное решение</t>
+  </si>
+  <si>
+    <t>Отчет создан: 29.09.2023 13:34:07</t>
+  </si>
+  <si>
+    <t>Результат: Решение найдено. Все ограничения и условия оптимальности выполнены.</t>
+  </si>
+  <si>
+    <t>Модуль поиска решения</t>
+  </si>
+  <si>
+    <t>Модуль: Поиск решения лин. задач симплекс-методом</t>
+  </si>
+  <si>
+    <t>Время решения: 0 секунд.</t>
+  </si>
+  <si>
+    <t>Число итераций: 2 Число подзадач: 0</t>
+  </si>
+  <si>
+    <t>Параметры поиска решения</t>
+  </si>
+  <si>
+    <t>Максимальное время Без пределов,  Число итераций Без пределов, Precision 0,000001, Использовать автоматическое масштабирование</t>
+  </si>
+  <si>
+    <t>Максимальное число подзадач Без пределов, Максимальное число целочисленных решений Без пределов, Целочисленное отклонение 1%, Считать неотрицательными</t>
+  </si>
+  <si>
+    <t>Ячейка целевой функции (Максимум)</t>
+  </si>
+  <si>
+    <t>Ячейка</t>
+  </si>
+  <si>
+    <t>Имя</t>
+  </si>
+  <si>
+    <t>Исходное значение</t>
+  </si>
+  <si>
+    <t>Окончательное значение</t>
+  </si>
+  <si>
+    <t>Ячейки переменных</t>
+  </si>
+  <si>
+    <t>Целочисленное</t>
+  </si>
+  <si>
+    <t>Значение ячейки</t>
+  </si>
+  <si>
+    <t>Формула</t>
+  </si>
+  <si>
+    <t>Состояние</t>
+  </si>
+  <si>
+    <t>Допуск</t>
+  </si>
+  <si>
+    <t>$D$4</t>
+  </si>
+  <si>
+    <t>$B$3</t>
+  </si>
+  <si>
+    <t>знач. x1</t>
+  </si>
+  <si>
+    <t>Продолжить</t>
+  </si>
+  <si>
+    <t>$C$3</t>
+  </si>
+  <si>
+    <t>знач. x2</t>
+  </si>
+  <si>
+    <t>$E$8</t>
+  </si>
+  <si>
+    <t>Рабочее время, чел.-ч лев.ч.</t>
+  </si>
+  <si>
+    <t>$E$8&lt;=$G$8</t>
+  </si>
+  <si>
+    <t>Привязка</t>
+  </si>
+  <si>
+    <t>$E$9</t>
+  </si>
+  <si>
+    <t>Кожа 1-го сорта лев.ч.</t>
+  </si>
+  <si>
+    <t>$E$9&lt;=$G$9</t>
+  </si>
+  <si>
+    <t>$E$10</t>
+  </si>
+  <si>
+    <t>Кожа 2-го сорта лев.ч.</t>
+  </si>
+  <si>
+    <t>$E$10&lt;=$G$10</t>
+  </si>
+  <si>
+    <t>Без привязки</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет об устойчивости</t>
+  </si>
+  <si>
+    <t>Отчет создан: 29.09.2023 13:34:50</t>
+  </si>
+  <si>
+    <t>Окончательное</t>
+  </si>
+  <si>
+    <t>Значение</t>
+  </si>
+  <si>
+    <t>Приведенн.</t>
+  </si>
+  <si>
+    <t>Стоимость</t>
+  </si>
+  <si>
+    <t>Целевая функция</t>
+  </si>
+  <si>
+    <t>Коэффициент</t>
+  </si>
+  <si>
+    <t>Допустимое</t>
+  </si>
+  <si>
+    <t>Увеличение</t>
+  </si>
+  <si>
+    <t>Уменьшение</t>
+  </si>
+  <si>
+    <t>Тень</t>
+  </si>
+  <si>
+    <t>Цена</t>
+  </si>
+  <si>
+    <t>Ограничение</t>
+  </si>
+  <si>
+    <t>Правая сторона</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Отчет о пределах</t>
+  </si>
+  <si>
+    <t>Переменная</t>
+  </si>
+  <si>
+    <t>Нижний</t>
+  </si>
+  <si>
+    <t>Предел</t>
+  </si>
+  <si>
+    <t>Результат</t>
+  </si>
+  <si>
+    <t>Верхний</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1219,6 +1466,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1246,7 +1501,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1254,11 +1509,60 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1282,12 +1586,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1297,13 +1607,24 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1643,155 +1964,155 @@
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="N1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
       <c r="N3" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="8">
         <v>1000</v>
       </c>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
         <v>1</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
       <c r="N4" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>500</v>
       </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="1">
         <v>1200</v>
       </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
       <c r="N5" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>1200</v>
       </c>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>50</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
         <v>40</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
       <c r="N6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1801,23 +2122,23 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="N1:P1"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
     <mergeCell ref="A1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="D1:G1"/>
@@ -1834,155 +2155,155 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="9" max="9" width="9.7109375" customWidth="1"/>
+    <col min="14" max="14" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="N1" s="10" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
       <c r="N2" s="1" t="s">
         <v>10</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9"/>
+      <c r="B3" s="8"/>
       <c r="C3" s="1">
         <v>1000</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>1</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
         <v>2</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="8"/>
       <c r="N3" t="s">
         <v>13</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="9">
+      <c r="P3" s="8">
         <v>1000</v>
       </c>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="1">
         <v>500</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>3</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
         <v>1</v>
       </c>
-      <c r="G4" s="9"/>
+      <c r="G4" s="8"/>
       <c r="N4" t="s">
         <v>15</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="9">
+      <c r="P4" s="8">
         <v>500</v>
       </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" s="1">
         <v>1200</v>
       </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="9"/>
+      <c r="G5" s="8"/>
       <c r="N5" t="s">
         <v>16</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="9">
+      <c r="P5" s="8">
         <v>1200</v>
       </c>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:17" ht="18" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
         <v>50</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
         <v>40</v>
       </c>
-      <c r="G6" s="9"/>
+      <c r="G6" s="8"/>
       <c r="N6" s="1" t="s">
         <v>17</v>
       </c>
@@ -1990,25 +2311,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="N8" s="10" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N8" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
+      <c r="O8" s="9"/>
+      <c r="P8" s="9"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="10" t="s">
         <v>26</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -2026,10 +2347,10 @@
       <c r="J9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K9" s="12" t="s">
+      <c r="K9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="12"/>
+      <c r="L9" s="14"/>
       <c r="N9" s="1" t="s">
         <v>10</v>
       </c>
@@ -2040,12 +2361,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="1">
         <v>50</v>
       </c>
@@ -2061,24 +2382,24 @@
       <c r="J10" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
       <c r="N10" t="s">
         <v>20</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P10" s="9">
+      <c r="P10" s="8">
         <v>1000</v>
       </c>
-      <c r="Q10" s="9"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="11">
-        <v>0</v>
-      </c>
-      <c r="B11" s="11"/>
+      <c r="Q10" s="8"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>0</v>
+      </c>
+      <c r="B11" s="13"/>
       <c r="C11" s="1" t="s">
         <v>29</v>
       </c>
@@ -2106,25 +2427,25 @@
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="12">
         <f>E11/F11</f>
         <v>1000</v>
       </c>
-      <c r="L11" s="13"/>
+      <c r="L11" s="12"/>
       <c r="N11" t="s">
         <v>21</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P11" s="9">
+      <c r="P11" s="8">
         <v>500</v>
       </c>
-      <c r="Q11" s="9"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="11"/>
+      <c r="Q11" s="8"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
@@ -2152,25 +2473,25 @@
       <c r="J12" s="3">
         <v>0</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="12">
         <f>E12/F12</f>
         <v>166.66666666666666</v>
       </c>
-      <c r="L12" s="13"/>
+      <c r="L12" s="12"/>
       <c r="N12" t="s">
         <v>22</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P12" s="9">
+      <c r="P12" s="8">
         <v>1200</v>
       </c>
-      <c r="Q12" s="9"/>
-    </row>
-    <row r="13" spans="1:17" ht="18" x14ac:dyDescent="0.3">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
+      <c r="Q12" s="8"/>
+    </row>
+    <row r="13" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="1" t="s">
         <v>31</v>
       </c>
@@ -2198,10 +2519,10 @@
       <c r="J13" s="1">
         <v>1</v>
       </c>
-      <c r="K13" s="14" t="s">
+      <c r="K13" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="L13" s="14"/>
+      <c r="L13" s="15"/>
       <c r="N13" s="1" t="s">
         <v>17</v>
       </c>
@@ -2209,13 +2530,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="8" t="s">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="8"/>
+      <c r="D14" s="10"/>
       <c r="E14" s="2" t="s">
         <v>36</v>
       </c>
@@ -2234,14 +2555,14 @@
       <c r="J14" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
       <c r="E15" s="1">
         <v>0</v>
       </c>
@@ -2265,14 +2586,14 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="11">
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>1</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
@@ -2302,15 +2623,15 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="12">
         <f>E16/G16</f>
         <v>500</v>
       </c>
-      <c r="L16" s="13"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+      <c r="L16" s="12"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
@@ -2340,15 +2661,15 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="12">
         <f>E17/G17</f>
         <v>500</v>
       </c>
-      <c r="L17" s="13"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
+      <c r="L17" s="12"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="1" t="s">
         <v>31</v>
       </c>
@@ -2378,26 +2699,26 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="12">
         <f>E18/G18</f>
         <v>1200</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="N18" s="15" t="s">
+      <c r="L18" s="12"/>
+      <c r="N18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="8" t="s">
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="8"/>
+      <c r="D19" s="10"/>
       <c r="E19" s="2" t="s">
         <v>36</v>
       </c>
@@ -2416,19 +2737,19 @@
       <c r="J19" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
       <c r="E20" s="1">
         <f>(E15*$F$12-$F15*E12)/$F$12</f>
         <v>8333.3333333333339</v>
@@ -2453,19 +2774,19 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="15"/>
-    </row>
-    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="11">
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="11"/>
+    </row>
+    <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
         <v>2</v>
       </c>
-      <c r="B21" s="11"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="1" t="s">
         <v>28</v>
       </c>
@@ -2495,19 +2816,19 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
+      <c r="L21" s="12"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="11"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
@@ -2537,19 +2858,19 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="K22" s="13" t="s">
+      <c r="K22" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
+      <c r="L22" s="12"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="11"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
       <c r="C23" s="1" t="s">
         <v>31</v>
       </c>
@@ -2579,23 +2900,23 @@
         <f>(J18*$G$16-J16*$G18)/$G$16</f>
         <v>1</v>
       </c>
-      <c r="K23" s="13" t="s">
+      <c r="K23" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="L23" s="13"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="15"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="8" t="s">
+      <c r="L23" s="12"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="11"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="8"/>
+      <c r="D24" s="10"/>
       <c r="E24" s="2" t="s">
         <v>36</v>
       </c>
@@ -2614,19 +2935,19 @@
       <c r="J24" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="11"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
       <c r="E25" s="5">
         <f>(E20*$G$16-E16*$G20)/$G$16</f>
         <v>20000</v>
@@ -2651,22 +2972,22 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="6"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="6"/>
@@ -2675,18 +2996,28 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="N18:R25"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L25"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L20"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
     <mergeCell ref="A11:B15"/>
     <mergeCell ref="A16:B20"/>
     <mergeCell ref="A21:B25"/>
@@ -2703,6 +3034,328 @@
     <mergeCell ref="K12:L12"/>
     <mergeCell ref="K13:L13"/>
     <mergeCell ref="K14:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K19:L20"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="N18:R25"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB38E0-1495-427A-B70D-7D750FA7B82B}">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="N1" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="8"/>
+      <c r="N2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q2" s="8"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="1">
+        <v>1000</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8">
+        <v>2</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="N3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P3" s="8">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="8"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="1">
+        <v>500</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="N4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="8">
+        <v>40</v>
+      </c>
+      <c r="Q4" s="8"/>
+    </row>
+    <row r="5" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="1">
+        <v>1200</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="N5" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>50</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8">
+        <v>40</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>20000</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="25">
+    <mergeCell ref="A9:G10"/>
+    <mergeCell ref="A15:C22"/>
+    <mergeCell ref="E15:G22"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:G6"/>
@@ -2717,321 +3370,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DB38E0-1495-427A-B70D-7D750FA7B82B}">
-  <dimension ref="A1:Q22"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="13.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="17" max="17" width="17.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="N1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="9"/>
-      <c r="N2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q2" s="9"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="1">
-        <v>1000</v>
-      </c>
-      <c r="D3" s="9">
-        <v>1</v>
-      </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9">
-        <v>2</v>
-      </c>
-      <c r="G3" s="9"/>
-      <c r="N3" t="s">
-        <v>46</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P3" s="9">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="9"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="1">
-        <v>500</v>
-      </c>
-      <c r="D4" s="9">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9">
-        <v>1</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="N4" t="s">
-        <v>47</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="9">
-        <v>40</v>
-      </c>
-      <c r="Q4" s="9"/>
-    </row>
-    <row r="5" spans="1:17" ht="18" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="1">
-        <v>1200</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="N5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="P5" s="9"/>
-      <c r="Q5" s="9"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9">
-        <v>50</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9">
-        <v>40</v>
-      </c>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="5">
-        <v>20000</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>14</v>
-      </c>
-      <c r="E12" s="1">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="E15" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-    </row>
-  </sheetData>
-  <mergeCells count="25">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
@@ -3040,23 +3378,863 @@
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="A9:G10"/>
-    <mergeCell ref="A15:C22"/>
-    <mergeCell ref="E15:G22"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5AE117-7DB2-49A0-A078-F783D7805C46}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="21">
+        <v>0</v>
+      </c>
+      <c r="E16" s="21">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="22">
+        <v>0</v>
+      </c>
+      <c r="E21" s="22">
+        <v>0</v>
+      </c>
+      <c r="F21" s="20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="21">
+        <v>0</v>
+      </c>
+      <c r="E22" s="21">
+        <v>500</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="G26" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D27" s="22">
+        <v>1000</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G27" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D28" s="22">
+        <v>500</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="G28" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29" s="21">
+        <v>500</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="18">
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1093A20-34B9-495C-A0EF-110FBC713931}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="20">
+        <v>0</v>
+      </c>
+      <c r="E9" s="20">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20">
+        <v>50</v>
+      </c>
+      <c r="G9" s="20">
+        <v>70.000000000000014</v>
+      </c>
+      <c r="H9" s="20">
+        <v>29.999999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="18">
+        <v>500</v>
+      </c>
+      <c r="E10" s="18">
+        <v>0</v>
+      </c>
+      <c r="F10" s="18">
+        <v>40</v>
+      </c>
+      <c r="G10" s="18">
+        <v>59.999999999999986</v>
+      </c>
+      <c r="H10" s="18">
+        <v>23.333333333333336</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" s="20">
+        <v>1000</v>
+      </c>
+      <c r="E15" s="20">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="F15" s="20">
+        <v>1000</v>
+      </c>
+      <c r="G15" s="20">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
+        <v>833.33333333333337</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="D16" s="20">
+        <v>500</v>
+      </c>
+      <c r="E16" s="20">
+        <v>11.999999999999996</v>
+      </c>
+      <c r="F16" s="20">
+        <v>500</v>
+      </c>
+      <c r="G16" s="20">
+        <v>2500</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17" s="18">
+        <v>500</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0</v>
+      </c>
+      <c r="F17" s="18">
+        <v>1200</v>
+      </c>
+      <c r="G17" s="18">
+        <v>1E+30</v>
+      </c>
+      <c r="H17" s="18">
+        <v>700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF7DB8B4-60E3-4ACD-A8D5-9F808351E431}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="21">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="23"/>
+      <c r="C11" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="23"/>
+      <c r="F11" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="24" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="22">
+        <v>0</v>
+      </c>
+      <c r="F13" s="22">
+        <v>0</v>
+      </c>
+      <c r="G13" s="22">
+        <v>20000</v>
+      </c>
+      <c r="I13" s="22">
+        <v>0</v>
+      </c>
+      <c r="J13" s="22">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D14" s="21">
+        <v>500</v>
+      </c>
+      <c r="F14" s="21">
+        <v>0</v>
+      </c>
+      <c r="G14" s="21">
+        <v>0</v>
+      </c>
+      <c r="I14" s="21">
+        <v>500</v>
+      </c>
+      <c r="J14" s="21">
+        <v>20000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE82FE51-E881-4FAB-A60D-34BE118350F5}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>500</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="1">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1">
+        <v>40</v>
+      </c>
+      <c r="D4" s="1">
+        <f>SUMPRODUCT($B$3:$C$3,B4:C4)</f>
+        <v>20000</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1">
+        <f>SUMPRODUCT($B$3:$C$3,C8:D8)</f>
+        <v>1000</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUMPRODUCT($B$3:$C$3,C9:D9)</f>
+        <v>500</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUMPRODUCT($B$3:$C$3,C10:D10)</f>
+        <v>500</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1200</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>